<commit_message>
fixing s1cDNA column in 09.08.20
</commit_message>
<xml_diff>
--- a/s1cDNASample/s1CDNASample_J.PLAGGENBERG_09.08.20.xlsx
+++ b/s1cDNASample/s1CDNASample_J.PLAGGENBERG_09.08.20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/s1cDNASample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B71B1CE-902A-9843-82CE-15645F57D6DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8E96E0-71C8-4D4D-892B-3404D673899D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="700" windowWidth="21440" windowHeight="18920" xr2:uid="{55392DBA-1BB3-7B40-9C7B-DE8352CE7AFF}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>polyAIsolationProtocol</t>
   </si>
   <si>
-    <t>s1Protocol</t>
-  </si>
-  <si>
     <t>roboticS1Prep</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>J.PLAGGENBERG</t>
+  </si>
+  <si>
+    <t>s1cDNAProtocol</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -469,781 +469,781 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
-        <v>12</v>
-      </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9">
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12">
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13">
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14">
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I14" t="b">
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15">
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
       </c>
       <c r="J15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16">
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17">
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18">
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19">
         <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I19" t="b">
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F20">
         <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I20" t="b">
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F21">
         <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I21" t="b">
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C22">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22">
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I22" t="b">
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F23">
         <v>22</v>
       </c>
       <c r="G23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F24">
         <v>23</v>
       </c>
       <c r="G24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I24" t="b">
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25">
         <v>24</v>
       </c>
       <c r="G25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I25" t="b">
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>